<commit_message>
updated conformance rules spreadsheet
</commit_message>
<xml_diff>
--- a/DataModel/USDM_ConformanceRules_SDR_Reference_ImplementationV1.xlsx
+++ b/DataModel/USDM_ConformanceRules_SDR_Reference_ImplementationV1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\viswesh.mb\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\indu.sekhar.sajja\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2675D9E-49B0-4DA2-BF4F-D145D645AEFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95E3EF4-89D1-4878-A976-8C6472A66510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A3ACD5DA-FA69-451A-83B4-E2EA342D7D58}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{A3ACD5DA-FA69-451A-83B4-E2EA342D7D58}"/>
   </bookViews>
   <sheets>
     <sheet name="StudyLevel" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3787" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3788" uniqueCount="345">
   <si>
     <t>StudyElement</t>
   </si>
@@ -1069,6 +1068,12 @@
   </si>
   <si>
     <t>amendment_effective_data</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Mandatory?</t>
   </si>
 </sst>
 </file>
@@ -1186,12 +1191,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1204,17 +1211,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1533,29 +1539,31 @@
   <dimension ref="A1:D116"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.140625" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" customWidth="1"/>
-    <col min="3" max="3" width="35.42578125" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="16383" max="16383" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.1796875" customWidth="1"/>
+    <col min="2" max="2" width="29.1796875" customWidth="1"/>
+    <col min="3" max="3" width="35.453125" customWidth="1"/>
+    <col min="4" max="4" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="16383" max="16383" width="9.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="6"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="8"/>
+      <c r="C1" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -1567,7 +1575,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1579,7 +1587,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1591,7 +1599,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1603,7 +1611,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1615,7 +1623,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -1627,7 +1635,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -1639,8 +1647,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1653,8 +1661,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="7"/>
       <c r="B10" s="1" t="s">
         <v>14</v>
       </c>
@@ -1665,8 +1673,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="7"/>
       <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
@@ -1677,8 +1685,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="13" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1691,8 +1699,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="13"/>
       <c r="B13" s="1" t="s">
         <v>18</v>
       </c>
@@ -1703,8 +1711,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="13"/>
       <c r="B14" s="1" t="s">
         <v>19</v>
       </c>
@@ -1715,8 +1723,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="13"/>
       <c r="B15" s="1" t="s">
         <v>20</v>
       </c>
@@ -1727,8 +1735,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="13"/>
       <c r="B16" s="1" t="s">
         <v>21</v>
       </c>
@@ -1739,7 +1747,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
@@ -1751,7 +1759,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
@@ -1763,8 +1771,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="7" t="s">
         <v>25</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1777,8 +1785,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="7"/>
       <c r="B20" s="1" t="s">
         <v>26</v>
       </c>
@@ -1789,8 +1797,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="7"/>
       <c r="B21" s="1" t="s">
         <v>27</v>
       </c>
@@ -1801,8 +1809,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="7"/>
       <c r="B22" s="1" t="s">
         <v>28</v>
       </c>
@@ -1813,8 +1821,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" s="7"/>
       <c r="B23" s="1" t="s">
         <v>30</v>
       </c>
@@ -1825,20 +1833,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" s="7"/>
       <c r="B24" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="5" t="s">
         <v>33</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" s="7"/>
       <c r="B25" s="1" t="s">
         <v>34</v>
       </c>
@@ -1849,8 +1857,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" s="7"/>
       <c r="B26" s="1" t="s">
         <v>35</v>
       </c>
@@ -1861,8 +1869,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" s="7"/>
       <c r="B27" s="1" t="s">
         <v>36</v>
       </c>
@@ -1873,7 +1881,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>37</v>
       </c>
@@ -1885,8 +1893,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" s="7" t="s">
         <v>39</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -1899,20 +1907,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" s="7"/>
       <c r="B30" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C30" s="5" t="s">
         <v>33</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" s="7"/>
       <c r="B31" s="1" t="s">
         <v>41</v>
       </c>
@@ -1923,8 +1931,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" s="7"/>
       <c r="B32" s="1" t="s">
         <v>43</v>
       </c>
@@ -1935,8 +1943,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" s="7"/>
       <c r="B33" s="1" t="s">
         <v>45</v>
       </c>
@@ -1947,8 +1955,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" s="7"/>
       <c r="B34" s="1" t="s">
         <v>47</v>
       </c>
@@ -1959,8 +1967,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" s="7"/>
       <c r="B35" s="1" t="s">
         <v>49</v>
       </c>
@@ -1971,32 +1979,32 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="5"/>
-      <c r="B36" s="13" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" s="7"/>
+      <c r="B36" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="C36" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
-      <c r="B37" s="13" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" s="7"/>
+      <c r="B37" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C37" s="12" t="s">
+      <c r="C37" s="5" t="s">
         <v>54</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="5"/>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38" s="7"/>
       <c r="B38" s="1" t="s">
         <v>55</v>
       </c>
@@ -2007,20 +2015,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="5"/>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" s="7"/>
       <c r="B39" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C39" s="12" t="s">
+      <c r="C39" s="5" t="s">
         <v>33</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
+    <row r="40" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="7" t="s">
         <v>57</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -2033,8 +2041,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="5"/>
+    <row r="41" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="7"/>
       <c r="B41" s="1" t="s">
         <v>58</v>
       </c>
@@ -2045,8 +2053,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="5"/>
+    <row r="42" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="7"/>
       <c r="B42" s="1" t="s">
         <v>59</v>
       </c>
@@ -2057,8 +2065,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="5"/>
+    <row r="43" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="7"/>
       <c r="B43" s="1" t="s">
         <v>61</v>
       </c>
@@ -2069,8 +2077,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A44" s="7" t="s">
         <v>58</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -2083,8 +2091,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
+    <row r="45" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="7"/>
       <c r="B45" s="1" t="s">
         <v>62</v>
       </c>
@@ -2095,20 +2103,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="5"/>
+    <row r="46" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="7"/>
       <c r="B46" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C46" s="12" t="s">
+      <c r="C46" s="5" t="s">
         <v>33</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="5"/>
+    <row r="47" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="7"/>
       <c r="B47" s="1" t="s">
         <v>64</v>
       </c>
@@ -2119,8 +2127,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="5"/>
+    <row r="48" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="7"/>
       <c r="B48" s="1" t="s">
         <v>65</v>
       </c>
@@ -2131,8 +2139,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="5"/>
+    <row r="49" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="7"/>
       <c r="B49" s="1" t="s">
         <v>66</v>
       </c>
@@ -2143,8 +2151,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="7" t="s">
+    <row r="50" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="9" t="s">
         <v>66</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -2157,20 +2165,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="8"/>
+    <row r="51" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="10"/>
       <c r="B51" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C51" s="12" t="s">
+      <c r="C51" s="5" t="s">
         <v>33</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="5" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A52" s="7" t="s">
         <v>68</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -2183,8 +2191,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="5"/>
+    <row r="53" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="7"/>
       <c r="B53" s="1" t="s">
         <v>69</v>
       </c>
@@ -2195,8 +2203,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="5"/>
+    <row r="54" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="7"/>
       <c r="B54" s="1" t="s">
         <v>70</v>
       </c>
@@ -2207,8 +2215,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="5"/>
+    <row r="55" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="7"/>
       <c r="B55" s="1" t="s">
         <v>71</v>
       </c>
@@ -2219,8 +2227,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="5"/>
+    <row r="56" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="7"/>
       <c r="B56" s="1" t="s">
         <v>73</v>
       </c>
@@ -2231,8 +2239,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="5" t="s">
+    <row r="57" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="7" t="s">
         <v>61</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -2245,32 +2253,32 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="5"/>
+    <row r="58" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="7"/>
       <c r="B58" s="1" t="s">
         <v>74</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D58" s="13" t="s">
+      <c r="D58" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="5"/>
+    <row r="59" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="7"/>
       <c r="B59" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D59" s="13" t="s">
+      <c r="D59" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="5"/>
+    <row r="60" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="7"/>
       <c r="B60" s="1" t="s">
         <v>76</v>
       </c>
@@ -2281,8 +2289,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="5"/>
+    <row r="61" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="7"/>
       <c r="B61" s="1" t="s">
         <v>77</v>
       </c>
@@ -2293,20 +2301,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="5"/>
+    <row r="62" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="7"/>
       <c r="B62" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C62" s="12" t="s">
+      <c r="C62" s="5" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="5" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A63" s="7" t="s">
         <v>79</v>
       </c>
       <c r="B63" s="1" t="s">
@@ -2319,8 +2327,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="5"/>
+    <row r="64" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="7"/>
       <c r="B64" s="1" t="s">
         <v>80</v>
       </c>
@@ -2331,8 +2339,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="5"/>
+    <row r="65" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="7"/>
       <c r="B65" s="1" t="s">
         <v>81</v>
       </c>
@@ -2343,8 +2351,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="5" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A66" s="7" t="s">
         <v>82</v>
       </c>
       <c r="B66" s="1" t="s">
@@ -2357,8 +2365,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="5"/>
+    <row r="67" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="7"/>
       <c r="B67" s="1" t="s">
         <v>80</v>
       </c>
@@ -2369,8 +2377,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="5"/>
+    <row r="68" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="7"/>
       <c r="B68" s="1" t="s">
         <v>83</v>
       </c>
@@ -2381,8 +2389,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="5" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A69" s="7" t="s">
         <v>84</v>
       </c>
       <c r="B69" s="1" t="s">
@@ -2395,8 +2403,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="5"/>
+    <row r="70" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="7"/>
       <c r="B70" s="1" t="s">
         <v>85</v>
       </c>
@@ -2407,8 +2415,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="5"/>
+    <row r="71" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="7"/>
       <c r="B71" s="1" t="s">
         <v>86</v>
       </c>
@@ -2419,20 +2427,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="5"/>
+    <row r="72" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="7"/>
       <c r="B72" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C72" s="12" t="s">
+      <c r="C72" s="5" t="s">
         <v>33</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="5" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A73" s="7" t="s">
         <v>89</v>
       </c>
       <c r="B73" s="1" t="s">
@@ -2445,8 +2453,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="5"/>
+    <row r="74" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="7"/>
       <c r="B74" s="1" t="s">
         <v>90</v>
       </c>
@@ -2457,20 +2465,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="5"/>
+    <row r="75" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="7"/>
       <c r="B75" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C75" s="12" t="s">
+      <c r="C75" s="5" t="s">
         <v>33</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="5"/>
+    <row r="76" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="7"/>
       <c r="B76" s="1" t="s">
         <v>92</v>
       </c>
@@ -2481,8 +2489,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="5" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A77" s="7" t="s">
         <v>93</v>
       </c>
       <c r="B77" s="1" t="s">
@@ -2495,8 +2503,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="5"/>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A78" s="7"/>
       <c r="B78" s="1" t="s">
         <v>94</v>
       </c>
@@ -2507,7 +2515,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="11" t="s">
         <v>95</v>
       </c>
@@ -2521,7 +2529,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="11"/>
       <c r="B80" s="1" t="s">
         <v>97</v>
@@ -2533,7 +2541,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" s="11"/>
       <c r="B81" s="1" t="s">
         <v>98</v>
@@ -2545,8 +2553,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="5" t="s">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A82" s="7" t="s">
         <v>100</v>
       </c>
       <c r="B82" s="1" t="s">
@@ -2559,8 +2567,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="5"/>
+    <row r="83" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A83" s="7"/>
       <c r="B83" s="1" t="s">
         <v>101</v>
       </c>
@@ -2571,8 +2579,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="5"/>
+    <row r="84" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A84" s="7"/>
       <c r="B84" s="1" t="s">
         <v>102</v>
       </c>
@@ -2583,8 +2591,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="5"/>
+    <row r="85" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A85" s="7"/>
       <c r="B85" s="1" t="s">
         <v>103</v>
       </c>
@@ -2595,8 +2603,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="5"/>
+    <row r="86" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A86" s="7"/>
       <c r="B86" s="1" t="s">
         <v>105</v>
       </c>
@@ -2607,8 +2615,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="5"/>
+    <row r="87" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="7"/>
       <c r="B87" s="1" t="s">
         <v>106</v>
       </c>
@@ -2619,8 +2627,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="9" t="s">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A88" s="12" t="s">
         <v>101</v>
       </c>
       <c r="B88" s="1" t="s">
@@ -2633,8 +2641,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="9"/>
+    <row r="89" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A89" s="12"/>
       <c r="B89" s="1" t="s">
         <v>107</v>
       </c>
@@ -2645,8 +2653,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="9"/>
+    <row r="90" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A90" s="12"/>
       <c r="B90" s="1" t="s">
         <v>108</v>
       </c>
@@ -2657,8 +2665,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="9"/>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A91" s="12"/>
       <c r="B91" s="1" t="s">
         <v>109</v>
       </c>
@@ -2669,8 +2677,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="9"/>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A92" s="12"/>
       <c r="B92" s="1" t="s">
         <v>111</v>
       </c>
@@ -2681,8 +2689,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="9"/>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A93" s="12"/>
       <c r="B93" s="1" t="s">
         <v>112</v>
       </c>
@@ -2693,8 +2701,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="9"/>
+    <row r="94" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A94" s="12"/>
       <c r="B94" s="1" t="s">
         <v>113</v>
       </c>
@@ -2705,8 +2713,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="10" t="s">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A95" s="13" t="s">
         <v>115</v>
       </c>
       <c r="B95" s="1" t="s">
@@ -2719,20 +2727,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="10"/>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A96" s="13"/>
       <c r="B96" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C96" s="12" t="s">
+      <c r="C96" s="5" t="s">
         <v>33</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="10"/>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A97" s="13"/>
       <c r="B97" s="1" t="s">
         <v>117</v>
       </c>
@@ -2743,8 +2751,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="10" t="s">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A98" s="13" t="s">
         <v>118</v>
       </c>
       <c r="B98" s="1" t="s">
@@ -2757,8 +2765,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="10"/>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A99" s="13"/>
       <c r="B99" s="1" t="s">
         <v>119</v>
       </c>
@@ -2769,8 +2777,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="10"/>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A100" s="13"/>
       <c r="B100" s="1" t="s">
         <v>120</v>
       </c>
@@ -2781,8 +2789,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="10"/>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A101" s="13"/>
       <c r="B101" s="1" t="s">
         <v>121</v>
       </c>
@@ -2793,8 +2801,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="10" t="s">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A102" s="13" t="s">
         <v>122</v>
       </c>
       <c r="B102" s="1" t="s">
@@ -2807,8 +2815,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="10"/>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A103" s="13"/>
       <c r="B103" s="1" t="s">
         <v>123</v>
       </c>
@@ -2819,8 +2827,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="10"/>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A104" s="13"/>
       <c r="B104" s="1" t="s">
         <v>124</v>
       </c>
@@ -2831,8 +2839,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="10"/>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A105" s="13"/>
       <c r="B105" s="1" t="s">
         <v>125</v>
       </c>
@@ -2843,8 +2851,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="10"/>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A106" s="13"/>
       <c r="B106" s="1" t="s">
         <v>126</v>
       </c>
@@ -2855,8 +2863,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="10"/>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A107" s="13"/>
       <c r="B107" s="1" t="s">
         <v>127</v>
       </c>
@@ -2867,8 +2875,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="5" t="s">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A108" s="7" t="s">
         <v>123</v>
       </c>
       <c r="B108" s="1" t="s">
@@ -2881,20 +2889,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="5"/>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A109" s="7"/>
       <c r="B109" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C109" s="12" t="s">
+      <c r="C109" s="5" t="s">
         <v>33</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="5"/>
+    <row r="110" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A110" s="7"/>
       <c r="B110" s="1" t="s">
         <v>83</v>
       </c>
@@ -2905,8 +2913,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="5" t="s">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A111" s="7" t="s">
         <v>125</v>
       </c>
       <c r="B111" s="1" t="s">
@@ -2919,8 +2927,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="5"/>
+    <row r="112" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A112" s="7"/>
       <c r="B112" s="1" t="s">
         <v>94</v>
       </c>
@@ -2931,8 +2939,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="5" t="s">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A113" s="7" t="s">
         <v>129</v>
       </c>
       <c r="B113" s="1" t="s">
@@ -2945,8 +2953,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="5"/>
+    <row r="114" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A114" s="7"/>
       <c r="B114" s="1" t="s">
         <v>130</v>
       </c>
@@ -2957,8 +2965,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="5"/>
+    <row r="115" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A115" s="7"/>
       <c r="B115" s="1" t="s">
         <v>131</v>
       </c>
@@ -2969,12 +2977,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="5"/>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A116" s="7"/>
       <c r="B116" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C116" s="12" t="s">
+      <c r="C116" s="5" t="s">
         <v>33</v>
       </c>
       <c r="D116" s="1" t="s">
@@ -2982,15 +2990,19 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D116" xr:uid="{D99043BE-1430-4060-BF1C-96B02CFC8CED}">
-    <filterColumn colId="0" showButton="0"/>
-    <filterColumn colId="2" showButton="0"/>
-  </autoFilter>
-  <mergeCells count="25">
+  <mergeCells count="24">
+    <mergeCell ref="A66:A68"/>
+    <mergeCell ref="A69:A72"/>
+    <mergeCell ref="A73:A76"/>
+    <mergeCell ref="A52:A56"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A19:A27"/>
+    <mergeCell ref="A29:A39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="A44:A49"/>
     <mergeCell ref="A108:A110"/>
     <mergeCell ref="A111:A112"/>
     <mergeCell ref="A113:A116"/>
-    <mergeCell ref="C1:D1"/>
     <mergeCell ref="A50:A51"/>
     <mergeCell ref="A79:A81"/>
     <mergeCell ref="A82:A87"/>
@@ -3003,36 +3015,27 @@
     <mergeCell ref="A12:A16"/>
     <mergeCell ref="A57:A62"/>
     <mergeCell ref="A63:A65"/>
-    <mergeCell ref="A66:A68"/>
-    <mergeCell ref="A69:A72"/>
-    <mergeCell ref="A73:A76"/>
-    <mergeCell ref="A52:A56"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A19:A27"/>
-    <mergeCell ref="A29:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="A44:A49"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C8" location="'StudyLevel'!A8:A10" display="List&lt;studyIdentifier&gt;" xr:uid="{D6C6EF37-1849-41EE-8780-B0106214E8B5}"/>
+    <hyperlink ref="C8" location="StudyLevel!A9:A11" display="List&lt;studyIdentifier&gt;" xr:uid="{D6C6EF37-1849-41EE-8780-B0106214E8B5}"/>
     <hyperlink ref="C7" location="Common!A2" display="code" xr:uid="{DF6A281D-19F6-4167-AF5F-30B961C22B02}"/>
     <hyperlink ref="C16" location="Common!A2" display="code" xr:uid="{92D24BA8-0BF0-4390-9A3B-31B29F733D22}"/>
-    <hyperlink ref="C11" location="'StudyLevel'!A11:A15" display="Organisation" xr:uid="{990CF59D-E24A-4B60-95F3-5735DF3D8B0B}"/>
+    <hyperlink ref="C11" location="StudyLevel!A12:A16" display="Organisation" xr:uid="{990CF59D-E24A-4B60-95F3-5735DF3D8B0B}"/>
     <hyperlink ref="C17" location="Common!A2" display="code" xr:uid="{69DB3301-9AC5-47C4-B4F3-F0B5EB556DF3}"/>
     <hyperlink ref="C30" location="Common!A2" display="code" xr:uid="{EC26F068-CDDA-4F91-BBF5-43377AD0A44B}"/>
     <hyperlink ref="C38" location="Common!A2" display="List&lt;code&gt;" xr:uid="{5BBD2D3D-6D16-4F74-B33A-5976B11E04F1}"/>
-    <hyperlink ref="C28" location="'StudyLevel'!A28:A38" display="List&lt;studyDesign&gt;" xr:uid="{C0EFD91F-6F73-4310-8529-C9B7FC94B96C}"/>
-    <hyperlink ref="C31" location="'StudyLevel'!A39:A42" display="List&lt;studyCell&gt;" xr:uid="{579CFE8F-AE35-4293-8851-24DC18D91618}"/>
-    <hyperlink ref="C32" location="'StudyLevel'!A62:A64" display="List&lt;Indication&gt;" xr:uid="{3ED0784C-BA1A-4C94-B84C-4B085C573337}"/>
-    <hyperlink ref="C33" location="'StudyLevel'!A65:A67" display="List&lt;InvestigationalIntervention&gt;" xr:uid="{7720A931-AC8B-4A5D-9D3E-5F1FB31411BF}"/>
-    <hyperlink ref="C34" location="'StudyLevel'!A68:A71" display="List&lt;Objective&gt;" xr:uid="{6A2AFF3E-3F70-43F7-A6A7-261259E2D393}"/>
-    <hyperlink ref="C35" location="'StudyLevel'!A76:A77" display="List&lt;studyDesignPopulation&gt;" xr:uid="{955A2131-2A24-4B7C-B082-A80DB8745000}"/>
-    <hyperlink ref="C41" location="'StudyLevel'!A43:A48" display="studyArm" xr:uid="{FB3B2BAC-8463-4C8F-9A36-29703D62C835}"/>
-    <hyperlink ref="C42" location="'StudyLevel'!A51:A55" display="List&lt;studyElement&gt;" xr:uid="{DB32F98B-02D8-4925-9CA5-62DBB00965A3}"/>
-    <hyperlink ref="C43" location="'StudyLevel'!A56:A61" display="studyEpoch" xr:uid="{F33A3F21-F08A-4027-A592-939DC870CC3E}"/>
+    <hyperlink ref="C28" location="StudyLevel!A29:A39" display="List&lt;studyDesign&gt;" xr:uid="{C0EFD91F-6F73-4310-8529-C9B7FC94B96C}"/>
+    <hyperlink ref="C31" location="StudyLevel!A40:A43" display="List&lt;studyCell&gt;" xr:uid="{579CFE8F-AE35-4293-8851-24DC18D91618}"/>
+    <hyperlink ref="C32" location="StudyLevel!A63:A65" display="List&lt;Indication&gt;" xr:uid="{3ED0784C-BA1A-4C94-B84C-4B085C573337}"/>
+    <hyperlink ref="C33" location="StudyLevel!A66:A68" display="List&lt;InvestigationalIntervention&gt;" xr:uid="{7720A931-AC8B-4A5D-9D3E-5F1FB31411BF}"/>
+    <hyperlink ref="C34" location="StudyLevel!A69:A72" display="List&lt;Objective&gt;" xr:uid="{6A2AFF3E-3F70-43F7-A6A7-261259E2D393}"/>
+    <hyperlink ref="C35" location="StudyLevel!A77:A78" display="List&lt;studyDesignPopulation&gt;" xr:uid="{955A2131-2A24-4B7C-B082-A80DB8745000}"/>
+    <hyperlink ref="C41" location="StudyLevel!A44:A49" display="studyArm" xr:uid="{FB3B2BAC-8463-4C8F-9A36-29703D62C835}"/>
+    <hyperlink ref="C42" location="StudyLevel!A52:A56" display="List&lt;studyElement&gt;" xr:uid="{DB32F98B-02D8-4925-9CA5-62DBB00965A3}"/>
+    <hyperlink ref="C43" location="StudyLevel!A57:A62" display="studyEpoch" xr:uid="{F33A3F21-F08A-4027-A592-939DC870CC3E}"/>
     <hyperlink ref="C55" location="Common!A7:A8" display="transitionRule" xr:uid="{6AE91DC0-FBE6-4823-952C-BE6E65CBBB7C}"/>
-    <hyperlink ref="C71" location="'StudyLevel'!A72:A75" display="List&lt;Endpoint&gt;" xr:uid="{03E0058E-25DD-4433-8E20-F176ED9A67DF}"/>
-    <hyperlink ref="C18" location="'StudyLevel'!A18:A26" display="List&lt;studyProtocolVersion&gt;" xr:uid="{EF848311-A24E-41F6-B560-3CF1BE6ACB95}"/>
+    <hyperlink ref="C71" location="StudyLevel!A73:A76" display="List&lt;Endpoint&gt;" xr:uid="{03E0058E-25DD-4433-8E20-F176ED9A67DF}"/>
+    <hyperlink ref="C18" location="StudyLevel!A19:A27" display="List&lt;studyProtocolVersion&gt;" xr:uid="{EF848311-A24E-41F6-B560-3CF1BE6ACB95}"/>
     <hyperlink ref="C64" location="Common!A2" display="List&lt;code&gt;" xr:uid="{CA27B9E5-2D88-4358-8B8D-FEDBC3E93F42}"/>
     <hyperlink ref="C67" location="Common!A2" display="List&lt;code&gt;" xr:uid="{5B0A1D69-14B9-47F0-BED2-2665E741BA89}"/>
     <hyperlink ref="C56" location="Common!A7:A8" display="transitionRule" xr:uid="{E9942144-BD23-431B-9C8C-9054310DACDC}"/>
@@ -3045,17 +3048,17 @@
     <hyperlink ref="C96" location="Common!A2" display="List&lt;code&gt;" xr:uid="{2F25345C-E9CA-4C3B-9C32-FEA0383FAFE1}"/>
     <hyperlink ref="C116" location="Common!A2" display="List&lt;code&gt;" xr:uid="{130CE16E-9D84-4200-BEDD-439788AB922A}"/>
     <hyperlink ref="C109" location="Common!A2" display="List&lt;code&gt;" xr:uid="{04C215F6-B5B5-4F81-BDCB-E6B723A4551E}"/>
-    <hyperlink ref="C36" location="'StudyLevel'!A78:A80" display="List&lt;Workflow&gt;" xr:uid="{0060A74B-9830-4105-9B17-DB17E2F450B6}"/>
-    <hyperlink ref="C37" location="'StudyLevel'!A101:A106" display="List&lt;Estimand&gt;" xr:uid="{0DBC0FF5-FAD1-4337-9702-E43EC8129681}"/>
-    <hyperlink ref="C49" location="'StudyLevel'!A49:A50" display="List&lt;studyArmType&gt;" xr:uid="{0190EBAE-CD3E-4680-B377-F96A6242F5C6}"/>
-    <hyperlink ref="C81" location="'StudyLevel'!A81:A86" display="List&lt;workflowItem&gt;" xr:uid="{AF960B24-9E2D-4BFE-9881-88416E069B18}"/>
-    <hyperlink ref="C83" location="'StudyLevel'!A87:A93" display="workflowItemActivity" xr:uid="{C61218C9-EC2E-425C-99E5-0A4E28697A92}"/>
+    <hyperlink ref="C36" location="StudyLevel!A79:A81" display="List&lt;Workflow&gt;" xr:uid="{0060A74B-9830-4105-9B17-DB17E2F450B6}"/>
+    <hyperlink ref="C37" location="StudyLevel!A102:A107" display="List&lt;Estimand&gt;" xr:uid="{0DBC0FF5-FAD1-4337-9702-E43EC8129681}"/>
+    <hyperlink ref="C49" location="StudyLevel!A50:A51" display="List&lt;studyArmType&gt;" xr:uid="{0190EBAE-CD3E-4680-B377-F96A6242F5C6}"/>
+    <hyperlink ref="C81" location="StudyLevel!A82:A87" display="List&lt;workflowItem&gt;" xr:uid="{AF960B24-9E2D-4BFE-9881-88416E069B18}"/>
+    <hyperlink ref="C83" location="StudyLevel!A88:A94" display="workflowItemActivity" xr:uid="{C61218C9-EC2E-425C-99E5-0A4E28697A92}"/>
     <hyperlink ref="C85" location="'Common'!A9:A18" display="Encounter" xr:uid="{A3C0362C-0A3F-4531-ADD2-7ACD871ABFA7}"/>
-    <hyperlink ref="C91" location="'StudyLevel'!A94:A96" display="List&lt;Procedure&gt;" xr:uid="{6001ED61-F098-4213-82D3-5BA3ABEEBBCA}"/>
-    <hyperlink ref="C94" location="'StudyLevel'!A97:A100" display="List&lt;studyData&gt;" xr:uid="{A56F9395-ABA5-4833-A116-804EF1B2EDEE}"/>
-    <hyperlink ref="C103" location="'StudyLevel'!A107:A109" display="treatment" xr:uid="{5E9A2057-4B68-4735-8A67-BD25ED90C86B}"/>
-    <hyperlink ref="C105" location="'StudyLevel'!A110:A111" display="analysisPopulation" xr:uid="{531EC587-94BB-4CCB-ACA2-BB93597F9BF8}"/>
-    <hyperlink ref="C107" location="'StudyLevel'!A112:A115" display="List&lt;InterCurrentEvent&gt;" xr:uid="{726DA2AF-A727-4234-8D5C-0E6AC79FC56E}"/>
+    <hyperlink ref="C91" location="StudyLevel!A95:A97" display="List&lt;Procedure&gt;" xr:uid="{6001ED61-F098-4213-82D3-5BA3ABEEBBCA}"/>
+    <hyperlink ref="C94" location="StudyLevel!A98:A101" display="List&lt;studyData&gt;" xr:uid="{A56F9395-ABA5-4833-A116-804EF1B2EDEE}"/>
+    <hyperlink ref="C103" location="StudyLevel!A108:A110" display="treatment" xr:uid="{5E9A2057-4B68-4735-8A67-BD25ED90C86B}"/>
+    <hyperlink ref="C105" location="StudyLevel!A111:A112" display="analysisPopulation" xr:uid="{531EC587-94BB-4CCB-ACA2-BB93597F9BF8}"/>
+    <hyperlink ref="C107" location="StudyLevel!A113:A116" display="List&lt;InterCurrentEvent&gt;" xr:uid="{726DA2AF-A727-4234-8D5C-0E6AC79FC56E}"/>
     <hyperlink ref="C106" location="'Common'!A9:A18" display="Encounter" xr:uid="{4B91DE3F-D8B8-44F0-867F-C9348BDE9926}"/>
     <hyperlink ref="C24" location="Common!A2" display="code" xr:uid="{263AF143-2A69-4804-977A-C2CBA95E796B}"/>
   </hyperlinks>
@@ -3069,22 +3072,22 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
+      <selection activeCell="A9" sqref="A9:A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1"/>
-    <col min="2" max="2" width="28.85546875" customWidth="1"/>
-    <col min="3" max="3" width="25.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.81640625" customWidth="1"/>
+    <col min="2" max="2" width="28.81640625" customWidth="1"/>
+    <col min="3" max="3" width="25.1796875" customWidth="1"/>
+    <col min="4" max="4" width="13.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="B1" s="6"/>
+      <c r="B1" s="8"/>
       <c r="C1" s="2" t="s">
         <v>134</v>
       </c>
@@ -3092,8 +3095,8 @@
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -3106,8 +3109,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="7"/>
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
@@ -3118,8 +3121,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="7"/>
       <c r="B4" s="1" t="s">
         <v>136</v>
       </c>
@@ -3130,8 +3133,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="7"/>
       <c r="B5" s="1" t="s">
         <v>137</v>
       </c>
@@ -3142,8 +3145,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="7"/>
       <c r="B6" s="1" t="s">
         <v>138</v>
       </c>
@@ -3154,8 +3157,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
         <v>72</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -3168,8 +3171,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="7"/>
       <c r="B8" s="1" t="s">
         <v>139</v>
       </c>
@@ -3180,8 +3183,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
         <v>104</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -3194,20 +3197,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="7"/>
       <c r="B10" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="5" t="s">
         <v>33</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="7"/>
       <c r="B11" s="1" t="s">
         <v>141</v>
       </c>
@@ -3218,20 +3221,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="7"/>
       <c r="B12" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="5" t="s">
         <v>33</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="7"/>
       <c r="B13" s="1" t="s">
         <v>143</v>
       </c>
@@ -3242,20 +3245,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="7"/>
       <c r="B14" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="5" t="s">
         <v>33</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="7"/>
       <c r="B15" s="1" t="s">
         <v>145</v>
       </c>
@@ -3266,8 +3269,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="7"/>
       <c r="B16" s="1" t="s">
         <v>146</v>
       </c>
@@ -3278,8 +3281,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="7"/>
       <c r="B17" s="1" t="s">
         <v>147</v>
       </c>
@@ -3290,8 +3293,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="7"/>
       <c r="B18" s="1" t="s">
         <v>148</v>
       </c>
@@ -3302,15 +3305,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="20" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="21" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="22" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="23" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="29" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="30" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="31" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
@@ -3338,34 +3341,34 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.140625" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="15.1796875" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1796875" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="30.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.54296875" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="17" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.26953125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="29" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="25.28515625" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="18.85546875" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="25.26953125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="18.81640625" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="25" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="14.85546875" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="19.5703125" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="23.85546875" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="23.140625" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="21.140625" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="19.42578125" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="18.5703125" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="27.5703125" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="17.28515625" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="16.42578125" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="14.42578125" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="14.81640625" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="19.54296875" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="23.81640625" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="23.1796875" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="21.1796875" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="19.453125" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="18.54296875" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="27.54296875" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="17.26953125" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="16.453125" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="14.453125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>149</v>
       </c>
@@ -3436,7 +3439,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>172</v>
       </c>
@@ -3507,7 +3510,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>172</v>
       </c>
@@ -3578,7 +3581,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>172</v>
       </c>
@@ -3649,7 +3652,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>172</v>
       </c>
@@ -3720,7 +3723,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>172</v>
       </c>
@@ -3791,7 +3794,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>172</v>
       </c>
@@ -3862,7 +3865,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>172</v>
       </c>
@@ -3933,7 +3936,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>172</v>
       </c>
@@ -4004,7 +4007,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>172</v>
       </c>
@@ -4075,7 +4078,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>172</v>
       </c>
@@ -4146,7 +4149,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>172</v>
       </c>
@@ -4217,7 +4220,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>172</v>
       </c>
@@ -4288,7 +4291,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>172</v>
       </c>
@@ -4359,7 +4362,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>172</v>
       </c>
@@ -4430,7 +4433,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>172</v>
       </c>
@@ -4501,7 +4504,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>172</v>
       </c>
@@ -4572,7 +4575,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>172</v>
       </c>
@@ -4643,7 +4646,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>172</v>
       </c>
@@ -4714,7 +4717,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>172</v>
       </c>
@@ -4785,7 +4788,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>172</v>
       </c>
@@ -4856,7 +4859,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>172</v>
       </c>
@@ -4927,7 +4930,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>172</v>
       </c>
@@ -4998,7 +5001,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>172</v>
       </c>
@@ -5069,7 +5072,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>172</v>
       </c>
@@ -5140,7 +5143,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>172</v>
       </c>
@@ -5211,7 +5214,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>172</v>
       </c>
@@ -5282,7 +5285,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>172</v>
       </c>
@@ -5353,7 +5356,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>172</v>
       </c>
@@ -5424,7 +5427,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>172</v>
       </c>
@@ -5495,7 +5498,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>172</v>
       </c>
@@ -5566,7 +5569,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>172</v>
       </c>
@@ -5637,7 +5640,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>172</v>
       </c>
@@ -5708,7 +5711,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>172</v>
       </c>
@@ -5779,7 +5782,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>172</v>
       </c>
@@ -5850,7 +5853,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>172</v>
       </c>
@@ -5921,7 +5924,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>172</v>
       </c>
@@ -5992,7 +5995,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>172</v>
       </c>
@@ -6063,7 +6066,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>172</v>
       </c>
@@ -6134,7 +6137,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>172</v>
       </c>
@@ -6205,7 +6208,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>172</v>
       </c>
@@ -6276,7 +6279,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>172</v>
       </c>
@@ -6347,7 +6350,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>172</v>
       </c>
@@ -6418,7 +6421,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>172</v>
       </c>
@@ -6489,7 +6492,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>172</v>
       </c>
@@ -6560,7 +6563,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>172</v>
       </c>
@@ -6631,7 +6634,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>172</v>
       </c>
@@ -6702,7 +6705,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>172</v>
       </c>
@@ -6773,7 +6776,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>172</v>
       </c>
@@ -6844,7 +6847,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>172</v>
       </c>
@@ -6915,7 +6918,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>172</v>
       </c>
@@ -6986,7 +6989,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>172</v>
       </c>
@@ -7057,7 +7060,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>172</v>
       </c>
@@ -7128,7 +7131,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>172</v>
       </c>
@@ -7199,7 +7202,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>172</v>
       </c>
@@ -7270,7 +7273,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>172</v>
       </c>
@@ -7341,7 +7344,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>172</v>
       </c>
@@ -7412,7 +7415,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>172</v>
       </c>
@@ -7483,7 +7486,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>172</v>
       </c>
@@ -7554,7 +7557,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>172</v>
       </c>
@@ -7625,7 +7628,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>172</v>
       </c>
@@ -7696,7 +7699,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>172</v>
       </c>
@@ -7767,7 +7770,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>172</v>
       </c>
@@ -7838,7 +7841,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>172</v>
       </c>
@@ -7909,7 +7912,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>172</v>
       </c>
@@ -7980,7 +7983,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>172</v>
       </c>
@@ -8051,7 +8054,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>172</v>
       </c>
@@ -8122,7 +8125,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>172</v>
       </c>
@@ -8193,7 +8196,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>172</v>
       </c>
@@ -8264,7 +8267,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>172</v>
       </c>
@@ -8335,7 +8338,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>172</v>
       </c>
@@ -8406,7 +8409,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>172</v>
       </c>
@@ -8477,7 +8480,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>172</v>
       </c>
@@ -8548,7 +8551,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>172</v>
       </c>
@@ -8619,7 +8622,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>172</v>
       </c>
@@ -8690,7 +8693,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="76" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>172</v>
       </c>
@@ -8761,7 +8764,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="77" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>172</v>
       </c>
@@ -8832,7 +8835,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="78" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>172</v>
       </c>
@@ -8903,7 +8906,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="79" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>172</v>
       </c>
@@ -8974,7 +8977,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="80" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>172</v>
       </c>
@@ -9045,7 +9048,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="81" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>172</v>
       </c>
@@ -9116,7 +9119,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="82" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>172</v>
       </c>
@@ -9187,7 +9190,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="83" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>172</v>
       </c>
@@ -9258,7 +9261,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="84" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>172</v>
       </c>
@@ -9329,7 +9332,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="85" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>172</v>
       </c>
@@ -9400,7 +9403,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="86" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>172</v>
       </c>
@@ -9471,7 +9474,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="87" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>172</v>
       </c>
@@ -9542,7 +9545,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="88" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>172</v>
       </c>
@@ -9613,7 +9616,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="89" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>172</v>
       </c>
@@ -9684,7 +9687,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="90" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>172</v>
       </c>
@@ -9755,7 +9758,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="91" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>172</v>
       </c>
@@ -9826,7 +9829,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="92" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>172</v>
       </c>
@@ -9897,7 +9900,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="93" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>172</v>
       </c>
@@ -9968,7 +9971,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="94" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>172</v>
       </c>
@@ -10039,7 +10042,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="95" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>172</v>
       </c>
@@ -10110,7 +10113,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="96" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>172</v>
       </c>
@@ -10181,7 +10184,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="97" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>172</v>
       </c>
@@ -10252,7 +10255,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="98" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>172</v>
       </c>
@@ -10323,7 +10326,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="99" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>172</v>
       </c>
@@ -10394,7 +10397,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="100" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>172</v>
       </c>
@@ -10465,7 +10468,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="101" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>172</v>
       </c>
@@ -10536,7 +10539,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="102" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>172</v>
       </c>
@@ -10607,7 +10610,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="103" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>172</v>
       </c>
@@ -10678,7 +10681,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="104" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>172</v>
       </c>
@@ -10749,7 +10752,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="105" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>172</v>
       </c>
@@ -10820,7 +10823,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="106" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>172</v>
       </c>
@@ -10891,7 +10894,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="107" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>172</v>
       </c>
@@ -10962,7 +10965,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="108" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>172</v>
       </c>
@@ -11033,7 +11036,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="109" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>172</v>
       </c>
@@ -11104,7 +11107,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="110" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>172</v>
       </c>
@@ -11175,7 +11178,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="111" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>172</v>
       </c>
@@ -11246,7 +11249,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="112" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>172</v>
       </c>
@@ -11317,7 +11320,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="113" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>172</v>
       </c>
@@ -11388,7 +11391,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="114" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>172</v>
       </c>
@@ -11459,7 +11462,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="115" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>172</v>
       </c>
@@ -11530,7 +11533,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="116" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>172</v>
       </c>
@@ -11601,7 +11604,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="117" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>172</v>
       </c>
@@ -11672,7 +11675,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="118" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>172</v>
       </c>
@@ -11743,7 +11746,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="119" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>172</v>
       </c>
@@ -11814,7 +11817,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="120" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>172</v>
       </c>
@@ -11885,7 +11888,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="121" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>172</v>
       </c>
@@ -11956,7 +11959,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="122" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>172</v>
       </c>
@@ -12027,7 +12030,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="123" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>172</v>
       </c>
@@ -12098,7 +12101,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="124" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>172</v>
       </c>
@@ -12169,7 +12172,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="125" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>172</v>
       </c>
@@ -12240,7 +12243,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="126" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>172</v>
       </c>
@@ -12311,7 +12314,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="127" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>172</v>
       </c>
@@ -12382,7 +12385,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="128" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>172</v>
       </c>
@@ -12453,7 +12456,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="129" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>172</v>
       </c>
@@ -12524,7 +12527,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="130" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>172</v>
       </c>
@@ -12595,7 +12598,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="131" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>172</v>
       </c>
@@ -12666,7 +12669,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="132" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>172</v>
       </c>
@@ -12737,7 +12740,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="133" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>172</v>
       </c>
@@ -12808,7 +12811,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="134" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>172</v>
       </c>
@@ -12879,7 +12882,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="135" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>172</v>
       </c>
@@ -12950,7 +12953,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="136" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>172</v>
       </c>
@@ -13021,7 +13024,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="137" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>172</v>
       </c>
@@ -13092,7 +13095,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="138" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>172</v>
       </c>
@@ -13163,7 +13166,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="139" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>172</v>
       </c>
@@ -13234,7 +13237,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="140" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>172</v>
       </c>
@@ -13305,7 +13308,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="141" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>172</v>
       </c>
@@ -13376,7 +13379,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="142" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>172</v>
       </c>
@@ -13447,7 +13450,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="143" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>172</v>
       </c>
@@ -13518,7 +13521,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="144" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>172</v>
       </c>
@@ -13589,7 +13592,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="145" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>172</v>
       </c>
@@ -13660,7 +13663,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="146" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>172</v>
       </c>
@@ -13731,7 +13734,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="147" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>172</v>
       </c>
@@ -13802,7 +13805,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="148" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>172</v>
       </c>
@@ -13873,7 +13876,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="149" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>172</v>
       </c>
@@ -13944,7 +13947,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="150" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>172</v>
       </c>
@@ -14015,7 +14018,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="151" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>172</v>
       </c>
@@ -14086,7 +14089,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="152" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>172</v>
       </c>
@@ -14157,7 +14160,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="153" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>172</v>
       </c>
@@ -14228,7 +14231,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="154" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>172</v>
       </c>
@@ -14299,7 +14302,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="155" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>172</v>
       </c>
@@ -14370,7 +14373,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="156" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>172</v>
       </c>
@@ -14441,7 +14444,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="157" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>172</v>
       </c>
@@ -14512,7 +14515,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="158" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>172</v>
       </c>
@@ -14583,7 +14586,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="159" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>172</v>
       </c>
@@ -14654,7 +14657,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="160" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>172</v>
       </c>
@@ -14725,7 +14728,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="161" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>172</v>
       </c>
@@ -14796,7 +14799,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="162" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>172</v>
       </c>
@@ -14874,6 +14877,25 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9ff55c19-750b-4d57-96fc-c7d80b080a4b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009F70ACD1D198BA4A93FC70EBD4D0E4F5" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="18b475abf70eecdc601daa3e136f5dd8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9ff55c19-750b-4d57-96fc-c7d80b080a4b" xmlns:ns3="a951cd76-9ac8-4a77-9c78-24aa33457680" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="74bfc7bfa49a56144affddbcba5bb63a" ns2:_="" ns3:_="">
     <xsd:import namespace="9ff55c19-750b-4d57-96fc-c7d80b080a4b"/>
@@ -15092,26 +15114,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9ff55c19-750b-4d57-96fc-c7d80b080a4b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7BF6920-7D60-46C8-8FE9-AA64B4468D49}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF55BEAE-E784-4B1F-B505-3E3A62064FF1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9ff55c19-750b-4d57-96fc-c7d80b080a4b"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7E78D44-13C1-49E4-985C-936A483EFDF6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15128,22 +15149,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF55BEAE-E784-4B1F-B505-3E3A62064FF1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9ff55c19-750b-4d57-96fc-c7d80b080a4b"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7BF6920-7D60-46C8-8FE9-AA64B4468D49}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>